<commit_message>
Specify config file on command line. Rearrange columns to keep 'Reports' last.
</commit_message>
<xml_diff>
--- a/tests/test_data.xlsx
+++ b/tests/test_data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\KJDELANEY\OneDrive - University of California, San Diego Health\Documents\GitHub\ExcelPostprocessor\tests\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="2" documentId="13_ncr:1_{328C55E0-FB99-4C85-8CD4-6CB6EEB0A8FC}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{D4BF12EE-572B-43B9-BF57-A8E5301F4BDF}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1801CF33-317A-401D-9CEE-FC3AB063FB9E}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="21465" windowHeight="8790" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="21465" windowHeight="8790" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Patients" sheetId="1" r:id="rId1"/>
@@ -35,16 +35,16 @@
     <t>`pH: 10.82 TDS 282.`</t>
   </si>
   <si>
-    <t>`Date of Exam: 12/25/2000. `LV EF MOD BP: 22% LVIDd: 2.23 cm Right Ventricle: TAPSE (2D): 2.24 cm RV S' Vmax: 2.25 m/s  MV e’ lateral: 2.26 m/s RVSP/PASP: 227 mmHg`</t>
-  </si>
-  <si>
-    <t>`Date of Exam: 12/25/1999. `LV EF MOD BP: 12% LVIDd: 1.23 cm Right Ventricle: TAPSE (2D): 1.24 cm RV S' Vmax: 1.25 m/s  MV e’ lateral: 1.26 m/s RVSP/PASP: 127 mmHg`</t>
-  </si>
-  <si>
-    <t>`Date of Exam: 12/25/1999. `LV EF MOD BP: 32% LVIDd: 3.23 cm Right Ventricle: TAPSE (2D): 3.24 cm RV S' Vmax: 3.25 m/s  MV e’ lateral: 3.26 m/s RVSP/PASP: 327 mmHg`</t>
-  </si>
-  <si>
     <t>REPORT</t>
+  </si>
+  <si>
+    <t>`Date of Exam: 12/25/1999. `LV EF MOD BP: 12% LVIDd: 1.23 cm Right Ventricle: TAPSE (2D): 1.24 cm RV S' Vmax: 1.25 m/s  MV e’ (lateral): 1.26 m/s RVSP/PASP: 127 mmHg`</t>
+  </si>
+  <si>
+    <t>`Date of Exam: 12/25/2000. `LV EF MOD BP: 22% LVIDd: 2.23 cm Right Ventricle: TAPSE (2D): 2.24 cm RV S' Vmax: 2.25 m/s  MV e’ (lateral): 2.26 m/s RVSP/PASP: 227 mmHg`</t>
+  </si>
+  <si>
+    <t>`Date of Exam: 12/25/1999. `LV EF MOD BP: 32% LVIDd: 3.23 cm Right Ventricle: TAPSE (2D): 3.24 cm RV S' Vmax: 3.25 m/s  MV e’ (lateral): 3.26 m/s RVSP/PASP: 327 mmHg`</t>
   </si>
 </sst>
 </file>
@@ -405,8 +405,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -419,7 +419,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="C1" s="2"/>
       <c r="D1" s="2"/>
@@ -437,7 +437,7 @@
         <v>2354</v>
       </c>
       <c r="B3" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
@@ -445,7 +445,7 @@
         <v>3456</v>
       </c>
       <c r="B4" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
     </row>
   </sheetData>
@@ -458,7 +458,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CEA3A826-9B8D-4E37-8CFF-3AC9A5AFB1E7}">
   <dimension ref="A1:C4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
@@ -472,7 +472,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="C1" s="2"/>
     </row>

</xml_diff>